<commit_message>
Deals with repeated entries.
</commit_message>
<xml_diff>
--- a/Lists/SBBE24Attendees.xlsx
+++ b/Lists/SBBE24Attendees.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B233"/>
+  <dimension ref="A1:B323"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -372,2782 +372,3862 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Constanza Clara Maubecin</t>
+          <t>Mario César C. de Pinna</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>cmaubecin@imbiv.unc.edu.ar</t>
+          <t>pinna@ib.usp.br</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>George Pacheco</t>
+          <t>Jose Alexandre Felizola Diniz Filho</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>george.pacheco@ibv.uio.no</t>
+          <t>diniz@ufg.br</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mylena Daiana Santander</t>
+          <t>Nelio Marco Vincenzo Bizzo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>mylena.santander@gmail.com</t>
+          <t>bizzo@unifesp.br</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Iara Patrícia Ferreira de Sousa</t>
+          <t>Nicolas Rocamundi</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>profiarapatricia@gmail.com</t>
+          <t>nicolasrocamundi@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Constância F. J. Ayres</t>
+          <t>Constanza Clara Maubecin</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>constancia.ayres@fiocruz.br</t>
+          <t>cmaubecin@imbiv.unc.edu.ar</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>JOAO PAULO SANTOS DA SILVA</t>
+          <t>Clarisse Palma da Silva</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>jpbiosilva@gmail.com</t>
+          <t>cpalma@unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BRENO BEZERRA JUST</t>
+          <t>Maria Emilia Yamamoto</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>brenojust99@gmail.com</t>
+          <t>emiliayamamoto@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ana Karoline da Nóbrega Nunes Alves</t>
+          <t>Luiz Eduardo Vieira Del Bem</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>anakarolinealves1@hotmail.com</t>
+          <t>levdelbem@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>José Eduardo Gomes De Oliveira</t>
+          <t>Fabricio Santos</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>zezinho20052005@gmail.com</t>
+          <t>fabricio-santos@ufmg.br</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Adrian Antonio Garda</t>
+          <t>Eduardo Tarazona</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>pseudis@gmail.com</t>
+          <t>edutars@icb.ufmg.br</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Gleyce Medeiros da Silva</t>
+          <t>Santiago Benitez Vieyra</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>gleycemedeiros96@gmail.com</t>
+          <t>santiagombv@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Paolla Gabryelle Cavalcante de Souza</t>
+          <t>Waldemir rosa</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>paollasouzac@gmail.com</t>
+          <t>waldemir.rosa@unila.edu.br</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Igor Peres Puertas dos Santos</t>
+          <t>George Pacheco</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>igorperesp@hotmail.com</t>
+          <t>george.pacheco@ibv.uio.no</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Graziela Santos Andrade</t>
+          <t>Andrea Pedrosa Harand</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>grazielaandrade.bio@gmail.com</t>
+          <t>andrea.harand@ufpe.br</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jonas Conduru Barros Neto</t>
+          <t>Kelly Zamudio</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>jonas.barrosneto@discente.univasf.edu.br</t>
+          <t>kelly.zamudio@austin.utexas.edu</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Ana Carolina Vilas Boas</t>
+          <t>Mylena Daiana Santander</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ananinanina@gmail.com</t>
+          <t>mylena.santander@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Henrique Batalha-Filho</t>
+          <t>Kateryna D Makov</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>henrique.batalha@outlook.com</t>
+          <t>makovakateryna@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Emilio de Lanna Neto</t>
+          <t>Prof. Dr. Frederico Henning</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>emiliolanna@gmail.com</t>
+          <t>fhenning@acd.ufrj.br</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Alessandra Selbach Schnadelbach</t>
+          <t>Ana Lúcia Tourinho</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>alessandra.schnadelbach@gmail.com</t>
+          <t>amtourinho@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Beatriz Santos De Brito</t>
+          <t>Thomaz Pinotti</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>beatrizbiologia2017@gmail.com</t>
+          <t>thomaz.pinoti@sund.ku.dk</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Isabelle Oliveira Lima Luz</t>
+          <t>Pedro Paulo Ferreira da Silva</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>isabelleluz@outlook.com.br</t>
+          <t>pedropaulofers@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Júlia de Lima Carvalho</t>
+          <t>Constância F. J. Ayres</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>julialima.carvalho18@gmail.com</t>
+          <t>constancia.ayres@fiocruz.br</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Fernanda Cavalcanti</t>
+          <t>JOAO PAULO SANTOS DA SILVA</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>fernanda.porifera@gmail.com</t>
+          <t>jpbiosilva@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Laysla Bomfim Adam</t>
+          <t>Ana Karoline da Nóbrega Nunes Alves</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>laysla.adam@gmail.com</t>
+          <t>anakarolinealves1@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Tami Mott</t>
+          <t>Sávio Torres de Farias</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>tami.mott@icbs.ufal.br</t>
+          <t>stfarias@yahoo.com.br</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>João Vitor Rodrigues Costa</t>
+          <t>BRENO BEZERRA JUST</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>vitorrodc@usp.br</t>
+          <t>brenojust99@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Sarah Waldschmidt da Cunha</t>
+          <t>Iara Patrícia Ferreira de Sousa</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>sarah.w.c2@gmail.com</t>
+          <t>profiarapatricia@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Esthefany Ovando De Mello</t>
+          <t>José Eduardo Gomes De Oliveira</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>esthefany0ovando@gmail.com</t>
+          <t>zezinho20052005@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Sarah Mângia Barros</t>
+          <t>Adrian Antonio Garda</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>sarahmangia@yahoo.com.br</t>
+          <t>pseudis@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Amanda Varago</t>
+          <t>Gleyce Medeiros da Silva</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>amandavarago021@gmail.com</t>
+          <t>gleycemedeiros96@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Evandro Douglas Moore de Lucena</t>
+          <t>Igor Peres Puertas dos Santos</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>douglas.moore@unesp.br</t>
+          <t>igorperesp@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Jeferson Vidart Ramos</t>
+          <t>Paolla Gabryelle Cavalcante de Souza</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>jeff.bioinfo@gmail.com</t>
+          <t>paollasouzac@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Larissa Bortoli de Souza</t>
+          <t>Aline Ghilardi</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>bortoli.larissa16@gmail.com</t>
+          <t>aline.ghilardi@ufrn.br</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Diego José Santana Silva</t>
+          <t>Graziela Santos Andrade</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>jose.santana@ufms.br</t>
+          <t>grazielaandrade.bio@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Matheus Sthanley Ferreira Firme</t>
+          <t>Ana Carolina Vilas Boas</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>fmatheuspba@gmail.com</t>
+          <t>ananinanina@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Guilherme Duarte</t>
+          <t>Bruno Cajado Almeida Gouveia</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>guilhermeduartepr@gmail.com</t>
+          <t>cajadobruno96@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Andressa Emanuele Johann</t>
+          <t>Emilio de Lanna Neto</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>johann_andressa@ufms.br</t>
+          <t>emiliolanna@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Vitória Infran De Morais</t>
+          <t>Henrique Batalha-Filho</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>vitoria.infran@ufms.br</t>
+          <t>henrique.batalha@outlook.com</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Lethícia Stéfany Barbosa Dias</t>
+          <t>Isabelle Oliveira Lima Luz</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>lethicia_dias@ufms.br</t>
+          <t>isabelleluz@outlook.com.br</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Aline Pedroso Lorenz</t>
+          <t>Alessandra Selbach Schnadelbach</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>aline.lorenz@ufms.br</t>
+          <t>alessandra.schnadelbach@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Akyel Kiffiner de França Mendonça</t>
+          <t>Beatriz Santos De Brito</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>a.kiffiner@gmail.com</t>
+          <t>beatrizbiologia2017@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Fernando Munir Lima Calarge</t>
+          <t>Júlia de Lima Carvalho</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>fernando.calarge@gmail.com</t>
+          <t>julialima.carvalho18@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Gecele Matos Paggi</t>
+          <t>Fernanda Cavalcanti</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>gecele.paggi@ufms.br</t>
+          <t>fernanda.porifera@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Bruna Da Rocha Maia</t>
+          <t>Laysla Bomfim Adam</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Brunadarochamaia@gmail.com</t>
+          <t>laysla.adam@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Renato Caparroz</t>
+          <t>Tami Mott</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>renatocz@yahoo.com.br</t>
+          <t>tami.mott@icbs.ufal.br</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Thiago Jose de Carvalho Andre</t>
+          <t>João Vitor Rodrigues Costa</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>thiago.andre@unb.br</t>
+          <t>vitorrodc@usp.br</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Marco Aurélio Mendes Elias</t>
+          <t>Bruna Da Rocha Maia</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>marcoelias.ecoevo@gmail.com</t>
+          <t>Brunadarochamaia@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Thannya Nascimento Soares</t>
+          <t>Roullien Henrique Martins Silva</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>tnsoares@ufg.br</t>
+          <t>roullien.silva@ufms.br</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Inês Soares de Menezes</t>
+          <t>Caio Lucas Barroso Nascimento Teixeira de Souza</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>iassismenezes@gmail.com</t>
+          <t>caiobarroso212@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Iderval da Silva Júnior Sobrinho</t>
+          <t>Larissa Bortoli de Souza</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>iderval_jr@yahoo.com</t>
+          <t>bortoli.larissa16@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Diogo Reis de Oliveira</t>
+          <t>Diego José Santana Silva</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>diogo.reisoliv@gmail.com</t>
+          <t>jose.santana@ufms.br</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Juliani Maciel dos Santos</t>
+          <t>Matheus Sthanley Ferreira Firme</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>juli.maciels@gmail.com</t>
+          <t>fmatheuspba@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Alejandra Bonilla Sánchez</t>
+          <t>Andressa Emanuele Johann</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>alejabonilla.sanchez@gmail.com</t>
+          <t>johann_andressa@ufms.br</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Lucca Azevedo Fanti</t>
+          <t>Gecele Matos Paggi</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>luccafanti2002@gmail.com</t>
+          <t>gecele.paggi@ufms.br</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Thaynara da Silva Lopes Lima</t>
+          <t>Fernando Munir Lima Calarge</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>thaynaralima_tsll@hotmail.com</t>
+          <t>fernando.calarge@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Carlos Robson Costa Cruz</t>
+          <t>Guilherme Duarte</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>cruz.carlosr21@gmail.com</t>
+          <t>guilhermeduartepr@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Letícia Monteiro</t>
+          <t>Leandro de Avelar Oliveira</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>leticiamonteiro.bio@gmail.com</t>
+          <t>leandro.avelar.bio@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Bruna Boizonave Andriola</t>
+          <t>Sarah Waldschmidt da Cunha</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>bruna.andriola@edu.pucrs.br</t>
+          <t>sarah.w.c2@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Gabriele Zenato Lazzari</t>
+          <t>Jeferson Vidart Ramos</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>gabriele.lazzari@edu.pucrs.br</t>
+          <t>jeff.bioinfo@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Marcia Holsbach Beltrame</t>
+          <t>Evandro Douglas Moore de Lucena</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>marcia.beltrame@ufrgs.br</t>
+          <t>douglas.moore@unesp.br</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>LAERCIO MOREIRA CARDOSO JUNIOR</t>
+          <t>Esthefany Ovando De Mello</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>laerciop53@gmail.com</t>
+          <t>esthefany0ovando@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Karoline Silva Zenato</t>
+          <t>Amanda Varago</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>karoline.szen@gmail.com</t>
+          <t>amandavarago021@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Juliana Cristine Fontana</t>
+          <t>Vitória Infran De Morais</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>julianacfontana@gmail.com</t>
+          <t>vitoria.infran@ufms.br</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Luana Sousa Soares</t>
+          <t>Lethícia Stéfany Barbosa Dias</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>lusousa.soares11@gmail.com</t>
+          <t>lethicia_dias@ufms.br</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Maikel Varal</t>
+          <t>Akyel Kiffiner de França Mendonça</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>maikelvaral@yahoo.com.br</t>
+          <t>a.kiffiner@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>André Luís da Silva Zani</t>
+          <t>Sarah Mângia Barros</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>zani.andre@yahoo.com.br</t>
+          <t>sarahmangia@yahoo.com.br</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Matías Maximiliano Malleret</t>
+          <t>Aline Pedroso Lorenz</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>malleret2@gmail.com</t>
+          <t>aline.lorenz@ufms.br</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>ANDREIA CARINA TURCHETTO ZOLET</t>
+          <t>Mariana Nunes Menegat</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>aturchetto@gmail.com</t>
+          <t>marianamenegat@outlook.com</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Juliene Lopes Costa</t>
+          <t>Isabela Caroline Moura dos Santos</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>julopescosta.23@gmail.com</t>
+          <t>bela_carolinem@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Pâmela Giordani Vielmo</t>
+          <t>Ariely Loyane Garcia Soares</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>pamelavielmo@hotmail.com</t>
+          <t>soares.loyane@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Mateus sousa de almeida</t>
+          <t>Renato Caparroz</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>mateus_btec@hotmail.com</t>
+          <t>renatocz@yahoo.com.br</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Aldo Mellender de Araújo</t>
+          <t>Thiago Jose de Carvalho Andre</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>aldo1806@gmail.com</t>
+          <t>thiago.andre@unb.br</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Bruna Oliveira Missaggia</t>
+          <t>Patricia Sanae Sujii</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>bmissaggia@gmail.com</t>
+          <t>sujiips@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Paulyana dos Santos Moura</t>
+          <t>Fernando Pacheco Rodrigues</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>paulyanamoura@gmail.com</t>
+          <t>fprodrigues@unb.br</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Manuel Adrian Riveros Escalona</t>
+          <t>Lilian Gimenes Giugliano</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>manuelriveros72@hotmail.com</t>
+          <t>liliangiu@unb.br</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Lorena Sanches Vieira</t>
+          <t>Marco Aurélio Mendes Elias</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>lolly.vieirasa@gmail.com</t>
+          <t>marcoelias.ecoevo@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Alejandra Niño Reyes</t>
+          <t>Thannya Nascimento Soares</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>alejandra.reyes@edu.pucrs.br</t>
+          <t>tnsoares@ufg.br</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Marco Silva Gottschalk</t>
+          <t>João Carlos Nabout</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>marco.gottschalk@yahoo.com</t>
+          <t>jcnabout@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Monica Laner Blauth</t>
+          <t>Inês Soares de Menezes</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>blauth.monica@gmail.com</t>
+          <t>iassismenezes@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Mariana Nunes Menegat</t>
+          <t>Iderval da Silva Júnior Sobrinho</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>marianamenegat@outlook.com</t>
+          <t>iderval_jr@yahoo.com</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Joana Gehlen Tessaro</t>
+          <t>Diogo Reis de Oliveira</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>tessarojg@gmail.com</t>
+          <t>diogo.reisoliv@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Roger Henrique Dalcin</t>
+          <t>Juliani Maciel dos Santos</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>roger.dalcin@gmail.com</t>
+          <t>juli.maciels@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Manuella Cardoso Teixeira</t>
+          <t>Alejandra Bonilla Sánchez</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>manuella.mhc2@gmail.com</t>
+          <t>alejabonilla.sanchez@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Andrea Rita Marrero</t>
+          <t>Marcia Holsbach Beltrame</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>andrea.marrero@ufsc.br</t>
+          <t>marcia.beltrame@ufrgs.br</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Giovanna Hernandez Garcia</t>
+          <t>LAERCIO MOREIRA CARDOSO JUNIOR</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>giio.ufsc@gmail.com</t>
+          <t>laerciop53@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Luiza Kittel Chiká</t>
+          <t>Juliana Cristine Fontana</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>luizakittel@gmail.com</t>
+          <t>julianacfontana@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Antonio Felipe Pereira dos Santos</t>
+          <t>Lucca Azevedo Fanti</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>antonio.fps@hotmail.com</t>
+          <t>luccafanti2002@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Jéssica Sueli dos Santos Batista</t>
+          <t>Bruna Boizonave Andriola</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>jessica.ssb@grad.ufsc.br</t>
+          <t>bruna.andriola@edu.pucrs.br</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Alexandre do Sacramento Alves Anselmo</t>
+          <t>Carolina Prauchner Silva</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>alexandre.sa.anselmo@gmail.com</t>
+          <t>carol_prauchner@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Nicoli Taísi Ornaghi</t>
+          <t>Karoline Silva Zenato</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>ra134020@uem.br</t>
+          <t>karoline.szen@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Pamella Oliveira Fardin</t>
+          <t>Gabriele Zenato Lazzari</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>ra134937@uem.br</t>
+          <t>gabriele.lazzari@edu.pucrs.br</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Aparecido Soares da Silva Júnior</t>
+          <t>João Pedro Carmo Filgueiras</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>ra124357@uem.br</t>
+          <t>jcarmofilgueiras@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Wanderley Dantas dos Santos</t>
+          <t>Lorena Sanches Vieira</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>wdsantos@uem.br</t>
+          <t>lolly.vieirasa@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Vinicius Oliveira Miranda</t>
+          <t>Manuel Adrian Riveros Escalona</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>viny.olmiranda@gmail.com</t>
+          <t>manuelriveros72@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Luiz Gustavo Gutierrez Ferreira</t>
+          <t>Paulyana dos Santos Moura</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>luiz318guti@gmail.com</t>
+          <t>paulyanamoura@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Maria Eduarda Araujo Ribeiro</t>
+          <t>Cássio Hervé</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>ra130004@uem.br</t>
+          <t>cassioherve@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Luana Garcia Siqueira Da Silva</t>
+          <t>Alejandra Niño Reyes</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>ra133953@uem.br</t>
+          <t>alejandra.reyes@edu.pucrs.br</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Wes</t>
+          <t>Luana Sousa Soares</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>wesley94moraes@gmail.com</t>
+          <t>lusousa.soares11@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Rodrigo A. Torres</t>
+          <t>André Luís da Silva Zani</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>rodrigotorres@utfpr.edu.br</t>
+          <t>zani.andre@yahoo.com.br</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Fabiano Stefanello</t>
+          <t>Maikel Varal</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>stefanellof@gmail.com</t>
+          <t>maikelvaral@yahoo.com.br</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Wesley Gomes Bojarski</t>
+          <t>Carlos Robson Costa Cruz</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>wesleybojarski@gmail.com</t>
+          <t>cruz.carlosr21@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Lucas Szekut de Paula</t>
+          <t>Letícia Monteiro</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>lucasszekutdepaula@gmail.com</t>
+          <t>leticiamonteiro.bio@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Adler Dvorak Barboza</t>
+          <t>Thaynara da Silva Lopes Lima</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>adlerdvorak@gmail.com</t>
+          <t>thaynaralima_tsll@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Marcela Naomi Okabayashi da Silva</t>
+          <t>ANDREIA CARINA TURCHETTO ZOLET</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>marcela.naomi@ufpr.br</t>
+          <t>aturchetto@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Valéria Ribeiro Da Silva</t>
+          <t>Matías Maximiliano Malleret</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>valeriaribeirosilva1@outlook.com</t>
+          <t>malleret2@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>João Mateus Zepson Capucho</t>
+          <t>Aldo Mellender de Araújo</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>joao.capucho@ufpr.br</t>
+          <t>aldo1806@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Michele Bertoncello</t>
+          <t>Bruna Oliveira Missaggia</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>michelebertoncello146@gmail.com</t>
+          <t>bmissaggia@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Marcos Barbeitos</t>
+          <t>Mateus sousa de almeida</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>msbarbeitos@gmail.com</t>
+          <t>mateus_btec@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Desirrê Alexia Lourenço Petters Vandresen</t>
+          <t>Marcelo Henrique Schwade</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>desirre.petters@gmail.com</t>
+          <t>marceloh.schwade@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Maria Julia Michelini de Almeida</t>
+          <t>Juliene Lopes Costa</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>majumichelini@gmail.com</t>
+          <t>julopescosta.23@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Mayara Pereira Neves</t>
+          <t>Pâmela Giordani Vielmo</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>mayara-nevesbio@hotmail.com</t>
+          <t>pamelavielmo@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Ana Beatriz Viergbiski Schwitzner</t>
+          <t>ISABEL GOMES VIEIRA</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>anabeatrizviergbiskischwitzner@gmail.com</t>
+          <t>belgovieira@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Thais Neves</t>
+          <t>Juliana Cordeiro</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>thaisneves2366@gmail.com</t>
+          <t>jlncdr@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Izadora Moraes da Silva</t>
+          <t>Aléxia Vittória Dariva Tormen</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>moraesiza12@gmail.com</t>
+          <t>alexia.tormen@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Vic Sant'Ana dos Santos</t>
+          <t>Marco Silva Gottschalk</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>rachel.santana2302@gmail.com</t>
+          <t>marco.gottschalk@yahoo.com</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>VILMAR FERNANDO BUENO JUNIOR</t>
+          <t>Monica Laner Blauth</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>vilmarbueno_@hotmail.com</t>
+          <t>blauth.monica@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Elisa de Castro Wille Nonino</t>
+          <t>Joana Gehlen Tessaro</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>elisanonino00@gmail.com</t>
+          <t>tessarojg@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Vitória Sávio Buchi</t>
+          <t>Roger Henrique Dalcin</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>viccabuchi@gmail.com</t>
+          <t>roger.dalcin@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Rodrigo Barbosa Gonçalves</t>
+          <t>Manuella Cardoso Teixeira</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>goncalvesrb@gmail.com</t>
+          <t>manuella.mhc2@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Raiana Santiago da Costa</t>
+          <t>Andrea Rita Marrero</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>val_raiana@hotmail.com</t>
+          <t>andrea.marrero@ufsc.br</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Juliane Xavier</t>
+          <t>Jéssica Sueli dos Santos Batista</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>julianexavier57361@gmail.com</t>
+          <t>jessica.ssb@grad.ufsc.br</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>LUCAS KATSUMI ROCHA HINOSHITA</t>
+          <t>Gabriéli Luiza Steffens Knapp</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>katsumilucas@gmail.com</t>
+          <t>gabrieli_steffens-pzo@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Ricardo Lehtonen Rodrigues Souza</t>
+          <t>Edgar De Paula Guerreiro</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>lehtonen@ufpr.br</t>
+          <t>edgar.guerreiro@tutanota.com</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>João Vitor Mello Hortega</t>
+          <t>Luiza Kittel Chiká</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>joaovitormelloh@gmail.com</t>
+          <t>luizakittel@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Bruno Torquato</t>
+          <t>Anglia Lavinia Lopes Moreira</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>brunotorquato100@gmail.com</t>
+          <t>anglia.lopes@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Henrique Luiz Rieger</t>
+          <t>Lorenzo Driessen Cigognini</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>henriquerieger2001@gmail.com</t>
+          <t>lorenzocigognini@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Juliana Rosa Matias Ciccheto</t>
+          <t>Antonio Felipe Pereira dos Santos</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>cicchetoju@gmail.com</t>
+          <t>antonio.fps@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Ana Julia Possamai de Oliveira</t>
+          <t>Giovanna Hernandez Garcia</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>anaju.possamai@gmail.com</t>
+          <t>giio.ufsc@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Maria Vitoria Lima da Silva</t>
+          <t>Vinicius Oliveira Miranda</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>mariavitoriadelima020@gmail.com</t>
+          <t>viny.olmiranda@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Mariana Guolo Moschen</t>
+          <t>Henrique Batista Gomes da Silva</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>marianagmoschen17@gmail.com</t>
+          <t>ra130150@uem.br</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Alexandre Henrique Pedroso</t>
+          <t>Wanderley Dantas dos Santos</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>ahenriquepedroso@gmail.com</t>
+          <t>wdsantos@uem.br</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Thamyris Weber Pereira</t>
+          <t>Aparecido Soares da Silva Júnior</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>thamyweber@gmail.com</t>
+          <t>ra124357@uem.br</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Bruna Buss</t>
+          <t>Luiz Gustavo Gutierrez Ferreira</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>brunacarolinebuss@gmail.com</t>
+          <t>luiz318guti@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Arquimedes Paixão de Santana Filho</t>
+          <t>Pamella Oliveira Fardin</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>santana@ufpr.br</t>
+          <t>ra134937@uem.br</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Leonardo Ricardo Nunes</t>
+          <t>Rodrigo de Mello</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>leonardoricardo518@gmail.com</t>
+          <t>rdemellobr@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Matheus Igor Fontana</t>
+          <t>Wes</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>matheu-igor@hotmail.com</t>
+          <t>wesley94moraes@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Amanda Beatriz Loureiro</t>
+          <t>Luana Garcia Siqueira Da Silva</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>amandabeatrizloureiro@gmail.com</t>
+          <t>ra133953@uem.br</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Leonardo Tyskowski Felix</t>
+          <t>Maria Eduarda Araujo Ribeiro</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>leotyszko@gmail.com</t>
+          <t>ra130004@uem.br</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Pedro Natale Cavezzale Dias</t>
+          <t>Alexandre do Sacramento Alves Anselmo</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>pnatalecd@gmail.com</t>
+          <t>alexandre.sa.anselmo@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Vitória Ibane</t>
+          <t>Nicoli Taísi Ornaghi</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>viibane@outlook.com</t>
+          <t>ra134020@uem.br</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Letícia Caroline Chaves</t>
+          <t>Leonardo Rodrigues Tolardo</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>leticia.leticiacchaves@gmail.com</t>
+          <t>leonardorodriguestolardo@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Luís Gustavo da Conceição Galego</t>
+          <t>Rodrigo A. Torres</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>luis.galego@uftm.edu.br</t>
+          <t>rodrigotorres@utfpr.edu.br</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Ronielson Gaia Da Silva</t>
+          <t>Roberto Ferreira Artoni</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>ronielsongaia@hotmail.com</t>
+          <t>rfartoni@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Thieres Tayroni Martins da Silva</t>
+          <t>Fabiano Stefanello</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>thierestayroni@gmail.com</t>
+          <t>stefanellof@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Fernando Araujo Perini</t>
+          <t>Luana Vieira</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>faperini@ufmg.br</t>
+          <t>luanavieira.snow@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Henry Paul Granger Neto</t>
+          <t>Wesley Gomes Bojarski</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>hp.granger98@gmail.com</t>
+          <t>wesleybojarski@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Laura Mara Silva Pereira</t>
+          <t>Lucas Szekut de Paula</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>laura.marasp@gmail.com</t>
+          <t>lucasszekutdepaula@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Davi Barbalho Cavalcanti</t>
+          <t>Adler Dvorak Barboza</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>barbalhodavi123@gmail.com</t>
+          <t>adlerdvorak@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Patricia Sanae Sujii</t>
+          <t>Marcela Naomi Okabayashi da Silva</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>sujiips@gmail.com</t>
+          <t>marcela.naomi@ufpr.br</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>MATEUS CHAMONE BURGARELLI</t>
+          <t>Valéria Ribeiro Da Silva</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>mateuschamone95@gmail.com</t>
+          <t>valeriaribeirosilva1@outlook.com</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Isaac Rafael Freitas Borges</t>
+          <t>Luddy Searom Carias de Moraes</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>isaacborges966@gmail.com</t>
+          <t>luddysearom@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>ANA CECILIA HOLLER DEL PRETTE</t>
+          <t>Maria Julia Michelini de Almeida</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>anacecilia.holler@gmail.com</t>
+          <t>majumichelini@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Gabriel Costa Santos</t>
+          <t>Marcos Barbeitos</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>gabrielscosta90@gmail.com</t>
+          <t>msbarbeitos@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Origilene Bezerra Dantas</t>
+          <t>Desirrê Alexia Lourenço Petters Vandresen</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>origilenedantas@gmail.com</t>
+          <t>desirre.petters@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Ramon Moreira Fernandes</t>
+          <t>João Mateus Zepson Capucho</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>ramonmf360@gmail.com</t>
+          <t>joao.capucho@ufpr.br</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Welignton Clarindo</t>
+          <t>Michele Bertoncello</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>well.clarindo@ufv.br</t>
+          <t>michelebertoncello146@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Alessandro Marques De Oliveira</t>
+          <t>Fabricius Maia Chaves Bicalho Domingos</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>biolessandro@gmail.com</t>
+          <t>fabricius.domingos@ufpr.br</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Mariana Fonseca Rossi</t>
+          <t>Arquimedes Paixão de Santana Filho</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>mfonsecarossi@gmail.com</t>
+          <t>santana@ufpr.br</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>André Yves</t>
+          <t>Amanda Beatriz Loureiro</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>andreyves7@gmail.com</t>
+          <t>amandabeatrizloureiro@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Henrique José de Oliveira</t>
+          <t>Bruna Buss</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>henrique.bio22@gmail.com</t>
+          <t>brunacarolinebuss@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>João Pedro Almeida Caetano</t>
+          <t>Matheus Maciel Alcantara Salles</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>20201200051@pq.uenf.br</t>
+          <t>matheusmaciel.salles@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Yasmim Alvarenga</t>
+          <t>Pedro Natale Cavezzale Dias</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>y.alvarenga.abreu@gmail.com</t>
+          <t>pnatalecd@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Juliana Lopes De Lima</t>
+          <t>Leonardo Tyskowski Felix</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>julianapv100@gmail.com</t>
+          <t>leotyszko@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Ismar de Souza Carvalho</t>
+          <t>Alexandre Henrique Pedroso</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>ismar@geologia.ufrj.br</t>
+          <t>ahenriquepedroso@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Clarice Assumpção da Costa</t>
+          <t>Thamyris Weber Pereira</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>assumpcao.clarice@gmail.com</t>
+          <t>thamyweber@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Luiza Silva Anselmini</t>
+          <t>Matheus Igor Fontana</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>miniansel.lu@gmail.com</t>
+          <t>matheu-igor@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Alessandra Pavan Lamarca</t>
+          <t>Leonardo Ricardo Nunes</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>pavanlamarca@gmail.com</t>
+          <t>leonardoricardo518@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Gabriela Ferreira Mota</t>
+          <t>Fernanda Witt Cidade</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>motafgabriela@gmail.com</t>
+          <t>fernandacidade@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Jose Ricardo Miras Mermudes</t>
+          <t>Mariana Guolo Moschen</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>jrmermudes@gmail.com</t>
+          <t>marianagmoschen17@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>José Mateus dos Santos</t>
+          <t>Ana Beatriz Viergbiski Schwitzner</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>mateussantosprof14@gmail.com</t>
+          <t>anabeatrizviergbiskischwitzner@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Davi Marques De Oliveira De Sá</t>
+          <t>Mayara Pereira Neves</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>ivadmarques48@gmail.com</t>
+          <t>mayara-nevesbio@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Claudia Augusta de Moraes Russo</t>
+          <t>Thais Neves</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>claurusso@hotmail.com</t>
+          <t>thaisneves2366@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Gabriel Henrique Nunes Rodrigues</t>
+          <t>Izadora Moraes da Silva</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>gabhengel@gmail.com</t>
+          <t>moraesiza12@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Alexandra Paris Toledo</t>
+          <t>Juliana Rosa Matias Ciccheto</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>alepariis@gmail.com</t>
+          <t>cicchetoju@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Lais Henriques de Mattos</t>
+          <t>Eric de Camargo Smidt</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>laishenriques91@gmail.com</t>
+          <t>ecsmidt@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Melissa Bars Closel</t>
+          <t>Maria Vitoria Lima da Silva</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>melissabars@gmail.com</t>
+          <t>mariavitoriadelima020@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Breno Michelon Seixas</t>
+          <t>Henrique Luiz Rieger</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>breno.mseixas@usp.br</t>
+          <t>henriquerieger2001@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Lucas Barcelos</t>
+          <t>Bruno Torquato</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>lucasabarcelos@gmail.com</t>
+          <t>brunotorquato100@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Thiago Takeshi Goto</t>
+          <t>João Vitor Mello Hortega</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>thi.takeshi@gmail.com</t>
+          <t>joaovitormelloh@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Danilo Camargo Fernandes</t>
+          <t>Ricardo Lehtonen Rodrigues Souza</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>danilo.fernandes@usp.br</t>
+          <t>lehtonen@ufpr.br</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Fernanda Biscaino Saluceste</t>
+          <t>LUCAS KATSUMI ROCHA HINOSHITA</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>fernanda.saluceste@unesp.br</t>
+          <t>katsumilucas@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Gustavo da Silva Ambrosio</t>
+          <t>Ana Julia Possamai de Oliveira</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>gustavo.ambrosio@unesp.br</t>
+          <t>anaju.possamai@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Gabriel Tofanelo Vanin</t>
+          <t>Rodrigo Barbosa Gonçalves</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>gabriel.vanin@unesp.br</t>
+          <t>goncalvesrb@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Leonardo Maurici Borges</t>
+          <t>Elisa de Castro Wille Nonino</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>aquitemcaqui@gmail.com</t>
+          <t>elisanonino00@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Rafael Fernandes Barduzzi</t>
+          <t>Vitória Sávio Buchi</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>rfbarduzzi@gmail.com</t>
+          <t>viccabuchi@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>João Pedro Fujita</t>
+          <t>Laura Laino da Costa</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>joaopedrofujita@estudante.ufscar.br</t>
+          <t>laura.costa231@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Victor Hugo Barbosa Pereira</t>
+          <t>Raiana Santiago da Costa</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>vhb.pereira@unesp.br</t>
+          <t>val_raiana@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Analice Gabrielle Marquezin Gomes</t>
+          <t>Juliane Xavier</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>analice.gabrielle@unesp.br</t>
+          <t>julianexavier57361@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Francisco Borges</t>
+          <t>Vic Sant'Ana dos Santos</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>fa.borges@unesp.br</t>
+          <t>rachel.santana2302@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Felipe Messias Leandro</t>
+          <t>VILMAR FERNANDO BUENO JUNIOR</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>felipe.messias@unesp.br</t>
+          <t>vilmarbueno_@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Pábulo Matheus Domiciano</t>
+          <t>Vitória Ibane</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>pabulodomiciano@gmail.com</t>
+          <t>viibane@outlook.com</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Pedro Henrique Pacheco Mosquini</t>
+          <t>Fernanda S. Caron</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>mosquiniphp@gmail.com</t>
+          <t>fernandadesouzacaron@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Tami da Costa Cacossi</t>
+          <t>Paulo Henrique Mueller</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>tamiccacossi@gmail.com</t>
+          <t>profmueller@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Vera Nisaka Solferini</t>
+          <t>Letícia Caroline Chaves</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>veras@unicamp.br</t>
+          <t>leticia.leticiacchaves@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Leonardo Duarte Santos</t>
+          <t>Heloise Tainá Sant’Anna</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>santosldbio@gmail.com</t>
+          <t>helo.taina.sa@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Henrique Vilela da Mata Bianchini</t>
+          <t>Luís Gustavo da Conceição Galego</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>h236891@dac.unicamp.br</t>
+          <t>luis.galego@uftm.edu.br</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Lucas Albuquerque dos Santos</t>
+          <t>Ronielson Gaia Da Silva</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>lucasabqsto@gmail.com</t>
+          <t>ronielsongaia@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Nicolle Souza Leto</t>
+          <t>Thieres Tayroni Martins da Silva</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>letonicolle@gmail.com</t>
+          <t>thierestayroni@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Diliane Harumi Yaguinuma</t>
+          <t>Henry Paul Granger Neto</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>diliane-harumi@hotmail.com</t>
+          <t>hp.granger98@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Tiago Benedito dos Santos</t>
+          <t>Laura Mara Silva Pereira</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>tiagobio02@yahoo.com.br</t>
+          <t>laura.marasp@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Jardel De Oliveira</t>
+          <t>Fernando Araujo Perini</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>jardel.oliveira90@hotmail.com</t>
+          <t>faperini@ufmg.br</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Ana Claudia Lessinger</t>
+          <t>Lucas Bleicher</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>lessinger@ufscar.br</t>
+          <t>lbleicher@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Miguel Piovesana Pereira Romeiro</t>
+          <t>Pammella Teixeira</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>miguelpromeiro@gmail.com</t>
+          <t>pammellateixeira@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Irene De Fátima Vieira De Moraes</t>
+          <t>Davi Barbalho Cavalcanti</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>irenef.vieiram@gmail.com</t>
+          <t>barbalhodavi123@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Eduardo Koerich Nery</t>
+          <t>MATEUS CHAMONE BURGARELLI</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>eduardo.k.nery@gmail.com</t>
+          <t>mateuschamone95@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>AMMIR YACOUB HELOU</t>
+          <t>Isaac Rafael Freitas Borges</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>ammir@usp.br</t>
+          <t>isaacborges966@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Letícia Wanderley Cavalcanti</t>
+          <t>ANA CECILIA HOLLER DEL PRETTE</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>letcavalcanti02@gmail.com</t>
+          <t>anacecilia.holler@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Gabriela Procópio Camacho</t>
+          <t>Gabriel Costa Santos</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>gpcamacho@usp.br</t>
+          <t>gabrielscosta90@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Nathália Caldeira Dias</t>
+          <t>Origilene Bezerra Dantas</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>caldeira.nathalia@gmail.com</t>
+          <t>origilenedantas@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Thiago Silva Loboda</t>
+          <t>Rafael Félix de Magalhães</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>loboda_bio@yahoo.com.br</t>
+          <t>rafaelmagalhaes@ufsj.edu.br</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Denis Calandriello Calio</t>
+          <t>Ramon Moreira Fernandes</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>denis.calan@gmail.com</t>
+          <t>ramonmf360@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Carlos Cristiano Simões Ferreira e Penha</t>
+          <t>Welignton Clarindo</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>cristianosf@usp.br</t>
+          <t>well.clarindo@ufv.br</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Ana Paula Becker</t>
+          <t>Alessandro Marques De Oliveira</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>ana.becker023@gmail.com</t>
+          <t>biolessandro@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Weverton dos Santos Azevedo</t>
+          <t>Mariana Fonseca Rossi</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>weverton.azevedo@hotmail.com</t>
+          <t>mfonsecarossi@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Rafaela Velloso Missagia</t>
+          <t>Henrique Caldeira Costa</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>rafaelamissagia@gmail.com</t>
+          <t>ccostah@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Marcelo Duarte</t>
+          <t>Henrique José de Oliveira</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>mduartes@usp.br</t>
+          <t>henrique.bio22@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Diogo Melo</t>
+          <t>André Yves</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>diogro@gmail.com</t>
+          <t>andreyves7@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Samuel Augusto Aguiar dos Anjos</t>
+          <t>João Pedro Almeida Caetano</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>sam_aanjos@usp.br</t>
+          <t>20201200051@pq.uenf.br</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Ana Paula Assis</t>
+          <t>Bruno Clarkson</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>paulaassis@ib.usp.br</t>
+          <t>brclarkson@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Joyce Rodrigues do Prado</t>
+          <t>Juliana Lopes De Lima</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>joyce.prado@usp.br</t>
+          <t>julianapv100@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>katarine nogueira norbertino</t>
+          <t>Yasmim Alvarenga</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>katarinenn@outlook.com</t>
+          <t>y.alvarenga.abreu@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Ivan Sergio Nunes Silva Filho</t>
+          <t>Davi Marques De Oliveira De Sá</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>ivan.nunes@unesp.br</t>
+          <t>ivadmarques48@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Erik Henrique de Lacerda Choueri</t>
+          <t>CLARISSA COIMBRA CANEDO</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>chouerik@gmail.com</t>
+          <t>clarissa.canedo@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Frederico Felizardo Barbosa</t>
+          <t>Miguel Godinho Alvares</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>fredericofb012@gmail.com</t>
+          <t>miguelgodinhoalvares@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Amanda Freitas Haase</t>
+          <t>Dener Soares Da Costa Junior</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>amandafreitashaase@gmail.com</t>
+          <t>denerdacosta12@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Felipe Arian de Andrade Araújo</t>
+          <t>Bruno Loreto de Aragão Pedroso</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>araujo.felipearian@gmail.com</t>
+          <t>bruno.loreto.aragao@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Gilmax Gonçalves Ferreira</t>
+          <t>Gabriel Henrique Nunes Rodrigues</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>gillmax88@gmail.com</t>
+          <t>gabhengel@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Thais Helena Condez</t>
+          <t>Claudia Augusta de Moraes Russo</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>thacondez@gmail.com</t>
+          <t>claurusso@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Pamela Maciel Cremonez</t>
+          <t>RAFAEL FILGUEIRA JORGE</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>pamelacremonez@gmail.com</t>
+          <t>rafajorgebio@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Isabella Fagundes Rosa Limão</t>
+          <t>Beatriz Mello Carvalho</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>isaarlimao@gmail.com</t>
+          <t>biaumello@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Gabriela Procopio Leite</t>
+          <t>Ana Carolina Martins Junqueira</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>gabrielaprocopio3@gmail.com</t>
+          <t>anacmj@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
+          <t>José Mateus dos Santos</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>mateussantosprof14@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Jose Ricardo Miras Mermudes</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>jrmermudes@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Carlos Eduardo Guerra Schrago</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>carlos.schrago@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Gabriela Ferreira Mota</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>motafgabriela@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Ismar de Souza Carvalho</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>ismar@geologia.ufrj.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Clarice Assumpção da Costa</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>assumpcao.clarice@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Ingrid Martins Machado Garcia Veiga</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>ingridgveiga@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Luiza Silva Anselmini</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>miniansel.lu@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>ALENA MAYO INIGUEZ</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>alenainiguez@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Lais Henriques de Mattos</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>laishenriques91@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Inês Corrêa Gonçalves</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>inescg.bio@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Lucas Pereira da Rocha</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>lucasrocha700@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Alexandra Paris Toledo</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>alepariis@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Alessandra Pavan Lamarca</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>pavanlamarca@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Luísa Andrade Mendes</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>mendesluisa1997@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Melissa Bars Closel</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>melissabars@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Breno Michelon Seixas</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>breno.mseixas@usp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Martín Rodrigo Escobar</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>martin.escobar@usp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Thiago Takeshi Goto</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>thi.takeshi@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Danilo Camargo Fernandes</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>danilo.fernandes@usp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>Lucas Barcelos</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>lucasabarcelos@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>Lígia Mouriño de Almeida Prado</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>ligia.prado@unesp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>Ana Malaghini de Abreu</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>anamalaghini9gold@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>Gabriel Tofanelo Vanin</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>gabriel.vanin@unesp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>Gustavo da Silva Ambrosio</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>gustavo.ambrosio@unesp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>Fernanda Biscaino Saluceste</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>fernanda.saluceste@unesp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>Leonardo Maurici Borges</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>aquitemcaqui@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>Rafael Fernandes Barduzzi</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>rfbarduzzi@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>Lucas Pereira Camargo</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>lucaspc@estudante.ufscar.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>João Pedro Fujita</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>joaopedrofujita@estudante.ufscar.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>Victor Hugo Barbosa Pereira</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>vhb.pereira@unesp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>Francisco Borges</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>fa.borges@unesp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>João Francisco Ponticelli Tottene</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>tott.joao@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>Felipe Messias Leandro</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>felipe.messias@unesp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>Analice Gabrielle Marquezin Gomes</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>analice.gabrielle@unesp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Luiza de Moraes Magaldi</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>luiza.magaldi@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>João Claudio de Sousa Nascimento</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>j.claudionasci@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>Pábulo Matheus Domiciano</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>pabulodomiciano@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>Nicolle Souza Leto</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>letonicolle@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>Pedro Henrique Pacheco Mosquini</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>mosquiniphp@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>Tami da Costa Cacossi</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>tamiccacossi@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>Leonardo Duarte Santos</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>santosldbio@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Vera Nisaka Solferini</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>veras@unicamp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Julia Nader Acquaviva</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>julianader95@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>Henrique Vilela da Mata Bianchini</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>h236891@dac.unicamp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>Paulo Aecyo Francisco da Silva</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>pauloaecyo_1997@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Beatriz Helena Macari Daros</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>beatrizdarosbio@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Pedro Paulo Goulart Taucci</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>pedrotaucce@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>Pedro Danel de Souza Ugarte</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>pedaugaso@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>Lucas Albuquerque dos Santos</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>lucasabqsto@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Amanda Lichtscheidl Graciadio</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>a265805@dac.unicamp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>Tiago Benedito dos Santos</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>tiagobio02@yahoo.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>Jardel De Oliveira</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>jardel.oliveira90@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>Diliane Harumi Yaguinuma</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>diliane-harumi@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>Ana Claudia Lessinger</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>lessinger@ufscar.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>Miguel Piovesana Pereira Romeiro</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>miguelpromeiro@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>Eduardo Koerich Nery</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>eduardo.k.nery@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>Irene De Fátima Vieira De Moraes</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>irenef.vieiram@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>Ana Paula Becker</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>ana.becker023@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>Marcelo Duarte</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>mduartes@usp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>Rafaela Velloso Missagia</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>rafaelamissagia@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>Diogo Melo</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>diogro@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>Weverton dos Santos Azevedo</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>weverton.azevedo@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>Ana Paula Assis</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>paulaassis@ib.usp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>Joyce Rodrigues do Prado</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>joyce.prado@usp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>Samuel Augusto Aguiar dos Anjos</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>sam_aanjos@usp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>katarine nogueira norbertino</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>katarinenn@outlook.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>Letícia Wanderley Cavalcanti</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>letcavalcanti02@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>Tábita Hünemeier</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>hunemeier@usp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>Gabriela Procópio Camacho</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>gpcamacho@usp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>Thiago Silva Loboda</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>loboda_bio@yahoo.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>Nathália Caldeira Dias</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>caldeira.nathalia@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>Carlos Cristiano Simões Ferreira e Penha</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>cristianosf@usp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>Denis Calandriello Calio</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>denis.calan@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>Tiago Bosisio Quental</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>tbquental@usp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>AMMIR YACOUB HELOU</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>ammir@usp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Ivan Sergio Nunes Silva Filho</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>ivan.nunes@unesp.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>Alexander Tamanini Mônico</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>alexandermonico@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>Fernanda de Pinho Werneck</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>fewerneck@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>Erik Henrique de Lacerda Choueri</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>chouerik@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>Esteban Diego Koch</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>edkoch17@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>Frederico Felizardo Barbosa</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>fredericofb012@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>Amanda Freitas Haase</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>amandafreitashaase@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>Felipe Arian de Andrade Araújo</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>araujo.felipearian@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>Gilmax Gonçalves Ferreira</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>gillmax88@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>Thais Helena Condez</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>thacondez@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>Pamela Maciel Cremonez</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>pamelacremonez@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>Isabella Fagundes Rosa Limão</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>isaarlimao@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>Jonas Conduru Barros Neto</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>jonas.barrosneto@discente.univasf.edu.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>Gabriela Procopio Leite</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>gabrielaprocopio3@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
           <t>Jonathan Murilo Andreu Conrado</t>
         </is>
       </c>
-      <c r="B233" t="inlineStr">
+      <c r="B323" t="inlineStr">
         <is>
           <t>jonathan.conrajo@gmail.com</t>
         </is>

</xml_diff>

<commit_message>
Deals better with repeated entries.
</commit_message>
<xml_diff>
--- a/Lists/SBBE24Attendees.xlsx
+++ b/Lists/SBBE24Attendees.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B323"/>
+  <dimension ref="A1:B333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,24 +420,24 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Constanza Clara Maubecin</t>
+          <t>Clarisse Palma da Silva</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>cmaubecin@imbiv.unc.edu.ar</t>
+          <t>cpalma@unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Clarisse Palma da Silva</t>
+          <t>Constanza Clara Maubecin</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>cpalma@unicamp.br</t>
+          <t>cmaubecin@imbiv.unc.edu.ar</t>
         </is>
       </c>
     </row>
@@ -804,72 +804,72 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Emilio de Lanna Neto</t>
+          <t>Henrique Batalha-Filho</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>emiliolanna@gmail.com</t>
+          <t>henrique.batalha@outlook.com</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Henrique Batalha-Filho</t>
+          <t>Isabelle Oliveira Lima Luz</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>henrique.batalha@outlook.com</t>
+          <t>isabelleluz@outlook.com.br</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Isabelle Oliveira Lima Luz</t>
+          <t>Júlia de Lima Carvalho</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>isabelleluz@outlook.com.br</t>
+          <t>julialima.carvalho18@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Alessandra Selbach Schnadelbach</t>
+          <t>Emilio de Lanna Neto</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>alessandra.schnadelbach@gmail.com</t>
+          <t>emiliolanna@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Beatriz Santos De Brito</t>
+          <t>Alessandra Selbach Schnadelbach</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>beatrizbiologia2017@gmail.com</t>
+          <t>alessandra.schnadelbach@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Júlia de Lima Carvalho</t>
+          <t>Beatriz Santos De Brito</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>julialima.carvalho18@gmail.com</t>
+          <t>beatrizbiologia2017@gmail.com</t>
         </is>
       </c>
     </row>
@@ -948,96 +948,96 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Caio Lucas Barroso Nascimento Teixeira de Souza</t>
+          <t>Andressa Emanuele Johann</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>caiobarroso212@gmail.com</t>
+          <t>johann_andressa@ufms.br</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Larissa Bortoli de Souza</t>
+          <t>Diego José Santana Silva</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>bortoli.larissa16@gmail.com</t>
+          <t>jose.santana@ufms.br</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Diego José Santana Silva</t>
+          <t>Caio Lucas Barroso Nascimento Teixeira de Souza</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>jose.santana@ufms.br</t>
+          <t>caiobarroso212@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Matheus Sthanley Ferreira Firme</t>
+          <t>Larissa Bortoli de Souza</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>fmatheuspba@gmail.com</t>
+          <t>bortoli.larissa16@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Andressa Emanuele Johann</t>
+          <t>Matheus Sthanley Ferreira Firme</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>johann_andressa@ufms.br</t>
+          <t>fmatheuspba@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Gecele Matos Paggi</t>
+          <t>Guilherme Duarte</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>gecele.paggi@ufms.br</t>
+          <t>guilhermeduartepr@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Fernando Munir Lima Calarge</t>
+          <t>Gecele Matos Paggi</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>fernando.calarge@gmail.com</t>
+          <t>gecele.paggi@ufms.br</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Guilherme Duarte</t>
+          <t>Fernando Munir Lima Calarge</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>guilhermeduartepr@gmail.com</t>
+          <t>fernando.calarge@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1104,60 +1104,60 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Amanda Varago</t>
+          <t>Vitória Infran De Morais</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>amandavarago021@gmail.com</t>
+          <t>vitoria.infran@ufms.br</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Vitória Infran De Morais</t>
+          <t>Lethícia Stéfany Barbosa Dias</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>vitoria.infran@ufms.br</t>
+          <t>lethicia_dias@ufms.br</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Lethícia Stéfany Barbosa Dias</t>
+          <t>Sarah Mângia Barros</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>lethicia_dias@ufms.br</t>
+          <t>sarahmangia@yahoo.com.br</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Akyel Kiffiner de França Mendonça</t>
+          <t>Amanda Varago</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>a.kiffiner@gmail.com</t>
+          <t>amandavarago021@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Sarah Mângia Barros</t>
+          <t>Akyel Kiffiner de França Mendonça</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>sarahmangia@yahoo.com.br</t>
+          <t>a.kiffiner@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1224,72 +1224,72 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Thiago Jose de Carvalho Andre</t>
+          <t>Frederico Hillesheim Horst</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>thiago.andre@unb.br</t>
+          <t>fredhorst7@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Patricia Sanae Sujii</t>
+          <t>Thiago Jose de Carvalho Andre</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>sujiips@gmail.com</t>
+          <t>thiago.andre@unb.br</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Fernando Pacheco Rodrigues</t>
+          <t>Patricia Sanae Sujii</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>fprodrigues@unb.br</t>
+          <t>sujiips@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Lilian Gimenes Giugliano</t>
+          <t>Fernando Pacheco Rodrigues</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>liliangiu@unb.br</t>
+          <t>fprodrigues@unb.br</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Marco Aurélio Mendes Elias</t>
+          <t>Lilian Gimenes Giugliano</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>marcoelias.ecoevo@gmail.com</t>
+          <t>liliangiu@unb.br</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Thannya Nascimento Soares</t>
+          <t>Marco Aurélio Mendes Elias</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>tnsoares@ufg.br</t>
+          <t>marcoelias.ecoevo@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1308,96 +1308,96 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Inês Soares de Menezes</t>
+          <t>Thannya Nascimento Soares</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>iassismenezes@gmail.com</t>
+          <t>tnsoares@ufg.br</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Iderval da Silva Júnior Sobrinho</t>
+          <t>Inês Soares de Menezes</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>iderval_jr@yahoo.com</t>
+          <t>iassismenezes@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Diogo Reis de Oliveira</t>
+          <t>Iderval da Silva Júnior Sobrinho</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>diogo.reisoliv@gmail.com</t>
+          <t>iderval_jr@yahoo.com</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Juliani Maciel dos Santos</t>
+          <t>Diogo Reis de Oliveira</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>juli.maciels@gmail.com</t>
+          <t>diogo.reisoliv@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Alejandra Bonilla Sánchez</t>
+          <t>Juliani Maciel dos Santos</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>alejabonilla.sanchez@gmail.com</t>
+          <t>juli.maciels@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Marcia Holsbach Beltrame</t>
+          <t>Alejandra Bonilla Sánchez</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>marcia.beltrame@ufrgs.br</t>
+          <t>alejabonilla.sanchez@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>LAERCIO MOREIRA CARDOSO JUNIOR</t>
+          <t>Marcia Holsbach Beltrame</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>laerciop53@gmail.com</t>
+          <t>marcia.beltrame@ufrgs.br</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Juliana Cristine Fontana</t>
+          <t>LAERCIO MOREIRA CARDOSO JUNIOR</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>julianacfontana@gmail.com</t>
+          <t>laerciop53@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1428,36 +1428,36 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Carolina Prauchner Silva</t>
+          <t>Karoline Silva Zenato</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>carol_prauchner@hotmail.com</t>
+          <t>karoline.szen@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Karoline Silva Zenato</t>
+          <t>Juliana Cristine Fontana</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>karoline.szen@gmail.com</t>
+          <t>julianacfontana@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Gabriele Zenato Lazzari</t>
+          <t>Carolina Prauchner Silva</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>gabriele.lazzari@edu.pucrs.br</t>
+          <t>carol_prauchner@hotmail.com</t>
         </is>
       </c>
     </row>
@@ -1476,120 +1476,120 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Lorena Sanches Vieira</t>
+          <t>Alejandra Niño Reyes</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>lolly.vieirasa@gmail.com</t>
+          <t>alejandra.reyes@edu.pucrs.br</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Manuel Adrian Riveros Escalona</t>
+          <t>Cássio Hervé</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>manuelriveros72@hotmail.com</t>
+          <t>cassioherve@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Paulyana dos Santos Moura</t>
+          <t>Manuel Adrian Riveros Escalona</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>paulyanamoura@gmail.com</t>
+          <t>manuelriveros72@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Cássio Hervé</t>
+          <t>Lorena Sanches Vieira</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>cassioherve@gmail.com</t>
+          <t>lolly.vieirasa@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Alejandra Niño Reyes</t>
+          <t>Gabriele Zenato Lazzari</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>alejandra.reyes@edu.pucrs.br</t>
+          <t>gabriele.lazzari@edu.pucrs.br</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Luana Sousa Soares</t>
+          <t>Paulyana dos Santos Moura</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>lusousa.soares11@gmail.com</t>
+          <t>paulyanamoura@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>André Luís da Silva Zani</t>
+          <t>Luana Sousa Soares</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>zani.andre@yahoo.com.br</t>
+          <t>lusousa.soares11@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Maikel Varal</t>
+          <t>André Luís da Silva Zani</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>maikelvaral@yahoo.com.br</t>
+          <t>zani.andre@yahoo.com.br</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Carlos Robson Costa Cruz</t>
+          <t>Maikel Varal</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>cruz.carlosr21@gmail.com</t>
+          <t>maikelvaral@yahoo.com.br</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Letícia Monteiro</t>
+          <t>Carlos Robson Costa Cruz</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>leticiamonteiro.bio@gmail.com</t>
+          <t>cruz.carlosr21@gmail.com</t>
         </is>
       </c>
     </row>
@@ -1608,552 +1608,552 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>ANDREIA CARINA TURCHETTO ZOLET</t>
+          <t>Letícia Monteiro</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>aturchetto@gmail.com</t>
+          <t>leticiamonteiro.bio@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Matías Maximiliano Malleret</t>
+          <t>ANDREIA CARINA TURCHETTO ZOLET</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>malleret2@gmail.com</t>
+          <t>aturchetto@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Aldo Mellender de Araújo</t>
+          <t>Matías Maximiliano Malleret</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>aldo1806@gmail.com</t>
+          <t>malleret2@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Bruna Oliveira Missaggia</t>
+          <t>Aldo Mellender de Araújo</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>bmissaggia@gmail.com</t>
+          <t>aldo1806@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Mateus sousa de almeida</t>
+          <t>Bruna Oliveira Missaggia</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>mateus_btec@hotmail.com</t>
+          <t>bmissaggia@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Marcelo Henrique Schwade</t>
+          <t>Juliene Lopes Costa</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>marceloh.schwade@gmail.com</t>
+          <t>julopescosta.23@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Juliene Lopes Costa</t>
+          <t>Pâmela Giordani Vielmo</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>julopescosta.23@gmail.com</t>
+          <t>pamelavielmo@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Pâmela Giordani Vielmo</t>
+          <t>Mateus sousa de almeida</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>pamelavielmo@hotmail.com</t>
+          <t>mateus_btec@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>ISABEL GOMES VIEIRA</t>
+          <t>Marcelo Henrique Schwade</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>belgovieira@gmail.com</t>
+          <t>marceloh.schwade@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Juliana Cordeiro</t>
+          <t>ISABEL GOMES VIEIRA</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>jlncdr@gmail.com</t>
+          <t>belgovieira@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Aléxia Vittória Dariva Tormen</t>
+          <t>Juliana Cordeiro</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>alexia.tormen@hotmail.com</t>
+          <t>jlncdr@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Marco Silva Gottschalk</t>
+          <t>Aléxia Vittória Dariva Tormen</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>marco.gottschalk@yahoo.com</t>
+          <t>alexia.tormen@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Monica Laner Blauth</t>
+          <t>Marco Silva Gottschalk</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>blauth.monica@gmail.com</t>
+          <t>marco.gottschalk@yahoo.com</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Joana Gehlen Tessaro</t>
+          <t>Monica Laner Blauth</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>tessarojg@gmail.com</t>
+          <t>blauth.monica@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Roger Henrique Dalcin</t>
+          <t>Joana Gehlen Tessaro</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>roger.dalcin@gmail.com</t>
+          <t>tessarojg@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Manuella Cardoso Teixeira</t>
+          <t>Roger Henrique Dalcin</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>manuella.mhc2@gmail.com</t>
+          <t>roger.dalcin@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Andrea Rita Marrero</t>
+          <t>Manuella Cardoso Teixeira</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>andrea.marrero@ufsc.br</t>
+          <t>manuella.mhc2@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Jéssica Sueli dos Santos Batista</t>
+          <t>Andrea Rita Marrero</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>jessica.ssb@grad.ufsc.br</t>
+          <t>andrea.marrero@ufsc.br</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Gabriéli Luiza Steffens Knapp</t>
+          <t>Jéssica Sueli dos Santos Batista</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>gabrieli_steffens-pzo@hotmail.com</t>
+          <t>jessica.ssb@grad.ufsc.br</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Edgar De Paula Guerreiro</t>
+          <t>Gabriéli Luiza Steffens Knapp</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>edgar.guerreiro@tutanota.com</t>
+          <t>gabrieli_steffens-pzo@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Luiza Kittel Chiká</t>
+          <t>Edgar De Paula Guerreiro</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>luizakittel@gmail.com</t>
+          <t>edgar.guerreiro@tutanota.com</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Anglia Lavinia Lopes Moreira</t>
+          <t>Luiza Kittel Chiká</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>anglia.lopes@gmail.com</t>
+          <t>luizakittel@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Lorenzo Driessen Cigognini</t>
+          <t>Anglia Lavinia Lopes Moreira</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>lorenzocigognini@gmail.com</t>
+          <t>anglia.lopes@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Antonio Felipe Pereira dos Santos</t>
+          <t>Lorenzo Driessen Cigognini</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>antonio.fps@hotmail.com</t>
+          <t>lorenzocigognini@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Giovanna Hernandez Garcia</t>
+          <t>Antonio Felipe Pereira dos Santos</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>giio.ufsc@gmail.com</t>
+          <t>antonio.fps@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Vinicius Oliveira Miranda</t>
+          <t>Giovanna Hernandez Garcia</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>viny.olmiranda@gmail.com</t>
+          <t>giio.ufsc@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Henrique Batista Gomes da Silva</t>
+          <t>Vinicius Oliveira Miranda</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>ra130150@uem.br</t>
+          <t>viny.olmiranda@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Wanderley Dantas dos Santos</t>
+          <t>Henrique Batista Gomes da Silva</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>wdsantos@uem.br</t>
+          <t>ra130150@uem.br</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Aparecido Soares da Silva Júnior</t>
+          <t>Wanderley Dantas dos Santos</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>ra124357@uem.br</t>
+          <t>wdsantos@uem.br</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Luiz Gustavo Gutierrez Ferreira</t>
+          <t>Aparecido Soares da Silva Júnior</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>luiz318guti@gmail.com</t>
+          <t>ra124357@uem.br</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Pamella Oliveira Fardin</t>
+          <t>Luiz Gustavo Gutierrez Ferreira</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>ra134937@uem.br</t>
+          <t>luiz318guti@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Rodrigo de Mello</t>
+          <t>Pamella Oliveira Fardin</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>rdemellobr@gmail.com</t>
+          <t>ra134937@uem.br</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Wes</t>
+          <t>Rodrigo de Mello</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>wesley94moraes@gmail.com</t>
+          <t>rdemellobr@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Luana Garcia Siqueira Da Silva</t>
+          <t>Wes</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>ra133953@uem.br</t>
+          <t>wesley94moraes@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Maria Eduarda Araujo Ribeiro</t>
+          <t>Luana Garcia Siqueira Da Silva</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>ra130004@uem.br</t>
+          <t>ra133953@uem.br</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Alexandre do Sacramento Alves Anselmo</t>
+          <t>Maria Eduarda Araujo Ribeiro</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>alexandre.sa.anselmo@gmail.com</t>
+          <t>ra130004@uem.br</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Nicoli Taísi Ornaghi</t>
+          <t>Alexandre do Sacramento Alves Anselmo</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>ra134020@uem.br</t>
+          <t>alexandre.sa.anselmo@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Leonardo Rodrigues Tolardo</t>
+          <t>Nicoli Taísi Ornaghi</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>leonardorodriguestolardo@gmail.com</t>
+          <t>ra134020@uem.br</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Rodrigo A. Torres</t>
+          <t>Leonardo Rodrigues Tolardo</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>rodrigotorres@utfpr.edu.br</t>
+          <t>leonardorodriguestolardo@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Roberto Ferreira Artoni</t>
+          <t>Rodrigo A. Torres</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>rfartoni@gmail.com</t>
+          <t>rodrigotorres@utfpr.edu.br</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Fabiano Stefanello</t>
+          <t>Roberto Ferreira Artoni</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>stefanellof@gmail.com</t>
+          <t>rfartoni@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Luana Vieira</t>
+          <t>Fabiano Stefanello</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>luanavieira.snow@gmail.com</t>
+          <t>stefanellof@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Wesley Gomes Bojarski</t>
+          <t>Luana Vieira</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>wesleybojarski@gmail.com</t>
+          <t>luanavieira.snow@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Lucas Szekut de Paula</t>
+          <t>Wesley Gomes Bojarski</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>lucasszekutdepaula@gmail.com</t>
+          <t>wesleybojarski@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Adler Dvorak Barboza</t>
+          <t>Lucas Szekut de Paula</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>adlerdvorak@gmail.com</t>
+          <t>lucasszekutdepaula@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Marcela Naomi Okabayashi da Silva</t>
+          <t>Adler Dvorak Barboza</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>marcela.naomi@ufpr.br</t>
+          <t>adlerdvorak@gmail.com</t>
         </is>
       </c>
     </row>
@@ -2172,120 +2172,120 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Luddy Searom Carias de Moraes</t>
+          <t>Marcela Naomi Okabayashi da Silva</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>luddysearom@gmail.com</t>
+          <t>marcela.naomi@ufpr.br</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Maria Julia Michelini de Almeida</t>
+          <t>Luddy Searom Carias de Moraes</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>majumichelini@gmail.com</t>
+          <t>luddysearom@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Marcos Barbeitos</t>
+          <t>João Mateus Zepson Capucho</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>msbarbeitos@gmail.com</t>
+          <t>joao.capucho@ufpr.br</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Desirrê Alexia Lourenço Petters Vandresen</t>
+          <t>Maria Julia Michelini de Almeida</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>desirre.petters@gmail.com</t>
+          <t>majumichelini@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>João Mateus Zepson Capucho</t>
+          <t>Michele Bertoncello</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>joao.capucho@ufpr.br</t>
+          <t>michelebertoncello146@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Michele Bertoncello</t>
+          <t>Marcos Barbeitos</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>michelebertoncello146@gmail.com</t>
+          <t>msbarbeitos@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Fabricius Maia Chaves Bicalho Domingos</t>
+          <t>Desirrê Alexia Lourenço Petters Vandresen</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>fabricius.domingos@ufpr.br</t>
+          <t>desirre.petters@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Arquimedes Paixão de Santana Filho</t>
+          <t>Fabricius Maia Chaves Bicalho Domingos</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>santana@ufpr.br</t>
+          <t>fabricius.domingos@ufpr.br</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Amanda Beatriz Loureiro</t>
+          <t>Arquimedes Paixão de Santana Filho</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>amandabeatrizloureiro@gmail.com</t>
+          <t>santana@ufpr.br</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Bruna Buss</t>
+          <t>Amanda Beatriz Loureiro</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>brunacarolinebuss@gmail.com</t>
+          <t>amandabeatrizloureiro@gmail.com</t>
         </is>
       </c>
     </row>
@@ -2304,1404 +2304,1404 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Pedro Natale Cavezzale Dias</t>
+          <t>Fernanda Freitas de Oliveira</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>pnatalecd@gmail.com</t>
+          <t>fernandaoliveira@ufpr.br</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Leonardo Tyskowski Felix</t>
+          <t>Pedro Natale Cavezzale Dias</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>leotyszko@gmail.com</t>
+          <t>pnatalecd@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Alexandre Henrique Pedroso</t>
+          <t>Leonardo Tyskowski Felix</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>ahenriquepedroso@gmail.com</t>
+          <t>leotyszko@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Thamyris Weber Pereira</t>
+          <t>Alexandre Henrique Pedroso</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>thamyweber@gmail.com</t>
+          <t>ahenriquepedroso@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Matheus Igor Fontana</t>
+          <t>Thamyris Weber Pereira</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>matheu-igor@hotmail.com</t>
+          <t>thamyweber@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Leonardo Ricardo Nunes</t>
+          <t>Fernanda Witt Cidade</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>leonardoricardo518@gmail.com</t>
+          <t>fernandacidade@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Fernanda Witt Cidade</t>
+          <t>Mariana Guolo Moschen</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>fernandacidade@gmail.com</t>
+          <t>marianagmoschen17@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Mariana Guolo Moschen</t>
+          <t>Leonardo Ricardo Nunes</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>marianagmoschen17@gmail.com</t>
+          <t>leonardoricardo518@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Ana Beatriz Viergbiski Schwitzner</t>
+          <t>Matheus Igor Fontana</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>anabeatrizviergbiskischwitzner@gmail.com</t>
+          <t>matheu-igor@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Mayara Pereira Neves</t>
+          <t>Talita Helen Bombardelli Gomig</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>mayara-nevesbio@hotmail.com</t>
+          <t>talitahbg@ufpr.br</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Thais Neves</t>
+          <t>Bruna Buss</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>thaisneves2366@gmail.com</t>
+          <t>brunacarolinebuss@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Izadora Moraes da Silva</t>
+          <t>VILMAR FERNANDO BUENO JUNIOR</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>moraesiza12@gmail.com</t>
+          <t>vilmarbueno_@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Juliana Rosa Matias Ciccheto</t>
+          <t>Vic Sant'Ana dos Santos</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>cicchetoju@gmail.com</t>
+          <t>rachel.santana2302@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Eric de Camargo Smidt</t>
+          <t>Rodrigo Barbosa Gonçalves</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>ecsmidt@gmail.com</t>
+          <t>goncalvesrb@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Maria Vitoria Lima da Silva</t>
+          <t>Raiana Santiago da Costa</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>mariavitoriadelima020@gmail.com</t>
+          <t>val_raiana@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Henrique Luiz Rieger</t>
+          <t>Juliane Xavier</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>henriquerieger2001@gmail.com</t>
+          <t>julianexavier57361@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Bruno Torquato</t>
+          <t>Elisa de Castro Wille Nonino</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>brunotorquato100@gmail.com</t>
+          <t>elisanonino00@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>João Vitor Mello Hortega</t>
+          <t>Laura Laino da Costa</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>joaovitormelloh@gmail.com</t>
+          <t>laura.costa231@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Ricardo Lehtonen Rodrigues Souza</t>
+          <t>Vitória Ibane</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>lehtonen@ufpr.br</t>
+          <t>viibane@outlook.com</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>LUCAS KATSUMI ROCHA HINOSHITA</t>
+          <t>Fernanda S. Caron</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>katsumilucas@gmail.com</t>
+          <t>fernandadesouzacaron@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Ana Julia Possamai de Oliveira</t>
+          <t>Nicole Isabelle Stocco</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>anaju.possamai@gmail.com</t>
+          <t>nicole.ufpr@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Rodrigo Barbosa Gonçalves</t>
+          <t>Vitória Sávio Buchi</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>goncalvesrb@gmail.com</t>
+          <t>viccabuchi@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Elisa de Castro Wille Nonino</t>
+          <t>Bruno Torquato</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>elisanonino00@gmail.com</t>
+          <t>brunotorquato100@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Vitória Sávio Buchi</t>
+          <t>João Vitor Mello Hortega</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>viccabuchi@gmail.com</t>
+          <t>joaovitormelloh@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Laura Laino da Costa</t>
+          <t>Ricardo Lehtonen Rodrigues Souza</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>laura.costa231@gmail.com</t>
+          <t>lehtonen@ufpr.br</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Raiana Santiago da Costa</t>
+          <t>LUCAS KATSUMI ROCHA HINOSHITA</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>val_raiana@hotmail.com</t>
+          <t>katsumilucas@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Juliane Xavier</t>
+          <t>Ana Julia Possamai de Oliveira</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>julianexavier57361@gmail.com</t>
+          <t>anaju.possamai@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Vic Sant'Ana dos Santos</t>
+          <t>Mayara Pereira Neves</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>rachel.santana2302@gmail.com</t>
+          <t>mayara-nevesbio@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>VILMAR FERNANDO BUENO JUNIOR</t>
+          <t>Thais Neves</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>vilmarbueno_@hotmail.com</t>
+          <t>thaisneves2366@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Vitória Ibane</t>
+          <t>Izadora Moraes da Silva</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>viibane@outlook.com</t>
+          <t>moraesiza12@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Fernanda S. Caron</t>
+          <t>Viviane da Silva-Pereira</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>fernandadesouzacaron@gmail.com</t>
+          <t>visilvapereira@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Paulo Henrique Mueller</t>
+          <t>Ana Beatriz Viergbiski Schwitzner</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>profmueller@gmail.com</t>
+          <t>anabeatrizviergbiskischwitzner@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Letícia Caroline Chaves</t>
+          <t>Juliana Rosa Matias Ciccheto</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>leticia.leticiacchaves@gmail.com</t>
+          <t>cicchetoju@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Heloise Tainá Sant’Anna</t>
+          <t>Eric de Camargo Smidt</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>helo.taina.sa@gmail.com</t>
+          <t>ecsmidt@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Luís Gustavo da Conceição Galego</t>
+          <t>Maria Vitoria Lima da Silva</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>luis.galego@uftm.edu.br</t>
+          <t>mariavitoriadelima020@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Ronielson Gaia Da Silva</t>
+          <t>Henrique Luiz Rieger</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>ronielsongaia@hotmail.com</t>
+          <t>henriquerieger2001@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Thieres Tayroni Martins da Silva</t>
+          <t>Paulo Henrique Mueller</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>thierestayroni@gmail.com</t>
+          <t>profmueller@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Henry Paul Granger Neto</t>
+          <t>Letícia Caroline Chaves</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>hp.granger98@gmail.com</t>
+          <t>leticia.leticiacchaves@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Laura Mara Silva Pereira</t>
+          <t>Heloise Tainá Sant’Anna</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>laura.marasp@gmail.com</t>
+          <t>helo.taina.sa@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Fernando Araujo Perini</t>
+          <t>Ronielson Gaia Da Silva</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>faperini@ufmg.br</t>
+          <t>ronielsongaia@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Lucas Bleicher</t>
+          <t>Luís Gustavo da Conceição Galego</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>lbleicher@gmail.com</t>
+          <t>luis.galego@uftm.edu.br</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Pammella Teixeira</t>
+          <t>Henry Paul Granger Neto</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>pammellateixeira@gmail.com</t>
+          <t>hp.granger98@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Davi Barbalho Cavalcanti</t>
+          <t>Laura Mara Silva Pereira</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>barbalhodavi123@gmail.com</t>
+          <t>laura.marasp@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>MATEUS CHAMONE BURGARELLI</t>
+          <t>Fernando Araujo Perini</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>mateuschamone95@gmail.com</t>
+          <t>faperini@ufmg.br</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Isaac Rafael Freitas Borges</t>
+          <t>Thieres Tayroni Martins da Silva</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>isaacborges966@gmail.com</t>
+          <t>thierestayroni@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>ANA CECILIA HOLLER DEL PRETTE</t>
+          <t>Lucas Bleicher</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>anacecilia.holler@gmail.com</t>
+          <t>lbleicher@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Gabriel Costa Santos</t>
+          <t>Davi Barbalho Cavalcanti</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>gabrielscosta90@gmail.com</t>
+          <t>barbalhodavi123@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Origilene Bezerra Dantas</t>
+          <t>Pammella Teixeira</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>origilenedantas@gmail.com</t>
+          <t>pammellateixeira@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Rafael Félix de Magalhães</t>
+          <t>MATEUS CHAMONE BURGARELLI</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>rafaelmagalhaes@ufsj.edu.br</t>
+          <t>mateuschamone95@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Ramon Moreira Fernandes</t>
+          <t>Isaac Rafael Freitas Borges</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>ramonmf360@gmail.com</t>
+          <t>isaacborges966@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Welignton Clarindo</t>
+          <t>ANA CECILIA HOLLER DEL PRETTE</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>well.clarindo@ufv.br</t>
+          <t>anacecilia.holler@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Alessandro Marques De Oliveira</t>
+          <t>Gabriel Costa Santos</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>biolessandro@gmail.com</t>
+          <t>gabrielscosta90@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Mariana Fonseca Rossi</t>
+          <t>Origilene Bezerra Dantas</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>mfonsecarossi@gmail.com</t>
+          <t>origilenedantas@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Henrique Caldeira Costa</t>
+          <t>Rafael Félix de Magalhães</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>ccostah@gmail.com</t>
+          <t>rafaelmagalhaes@ufsj.edu.br</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Henrique José de Oliveira</t>
+          <t>Ramon Moreira Fernandes</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>henrique.bio22@gmail.com</t>
+          <t>ramonmf360@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>André Yves</t>
+          <t>Welignton Clarindo</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>andreyves7@gmail.com</t>
+          <t>well.clarindo@ufv.br</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>João Pedro Almeida Caetano</t>
+          <t>Alessandro Marques De Oliveira</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>20201200051@pq.uenf.br</t>
+          <t>biolessandro@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Bruno Clarkson</t>
+          <t>Mariana Fonseca Rossi</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>brclarkson@gmail.com</t>
+          <t>mfonsecarossi@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Juliana Lopes De Lima</t>
+          <t>Henrique Caldeira Costa</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>julianapv100@gmail.com</t>
+          <t>ccostah@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Yasmim Alvarenga</t>
+          <t>Henrique José de Oliveira</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>y.alvarenga.abreu@gmail.com</t>
+          <t>henrique.bio22@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Davi Marques De Oliveira De Sá</t>
+          <t>André Yves</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>ivadmarques48@gmail.com</t>
+          <t>andreyves7@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>CLARISSA COIMBRA CANEDO</t>
+          <t>João Pedro Almeida Caetano</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>clarissa.canedo@gmail.com</t>
+          <t>20201200051@pq.uenf.br</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Miguel Godinho Alvares</t>
+          <t>Bruno Clarkson</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>miguelgodinhoalvares@gmail.com</t>
+          <t>brclarkson@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Dener Soares Da Costa Junior</t>
+          <t>Juliana Lopes De Lima</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>denerdacosta12@gmail.com</t>
+          <t>julianapv100@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Bruno Loreto de Aragão Pedroso</t>
+          <t>Yasmim Alvarenga</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>bruno.loreto.aragao@hotmail.com</t>
+          <t>y.alvarenga.abreu@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Gabriel Henrique Nunes Rodrigues</t>
+          <t>Comissão Avaliadora</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>gabhengel@gmail.com</t>
+          <t>angela_portella@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Claudia Augusta de Moraes Russo</t>
+          <t>RAFAEL FILGUEIRA JORGE</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>claurusso@hotmail.com</t>
+          <t>rafajorgebio@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>RAFAEL FILGUEIRA JORGE</t>
+          <t>Ana Carolina Martins Junqueira</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>rafajorgebio@gmail.com</t>
+          <t>anacmj@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Beatriz Mello Carvalho</t>
+          <t>José Mateus dos Santos</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>biaumello@gmail.com</t>
+          <t>mateussantosprof14@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Ana Carolina Martins Junqueira</t>
+          <t>Jose Ricardo Miras Mermudes</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>anacmj@gmail.com</t>
+          <t>jrmermudes@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>José Mateus dos Santos</t>
+          <t>Davi Marques De Oliveira De Sá</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>mateussantosprof14@gmail.com</t>
+          <t>ivadmarques48@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Jose Ricardo Miras Mermudes</t>
+          <t>CLARISSA COIMBRA CANEDO</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>jrmermudes@gmail.com</t>
+          <t>clarissa.canedo@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Carlos Eduardo Guerra Schrago</t>
+          <t>Miguel Godinho Alvares</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>carlos.schrago@gmail.com</t>
+          <t>miguelgodinhoalvares@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Gabriela Ferreira Mota</t>
+          <t>Dener Soares Da Costa Junior</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>motafgabriela@gmail.com</t>
+          <t>denerdacosta12@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Ismar de Souza Carvalho</t>
+          <t>Bruno Loreto de Aragão Pedroso</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>ismar@geologia.ufrj.br</t>
+          <t>bruno.loreto.aragao@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>Clarice Assumpção da Costa</t>
+          <t>Gabriel Henrique Nunes Rodrigues</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>assumpcao.clarice@gmail.com</t>
+          <t>gabhengel@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Ingrid Martins Machado Garcia Veiga</t>
+          <t>Claudia Augusta de Moraes Russo</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>ingridgveiga@gmail.com</t>
+          <t>claurusso@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Luiza Silva Anselmini</t>
+          <t>Carlos Eduardo Guerra Schrago</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>miniansel.lu@gmail.com</t>
+          <t>carlos.schrago@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>ALENA MAYO INIGUEZ</t>
+          <t>Beatriz Mello Carvalho</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>alenainiguez@gmail.com</t>
+          <t>biaumello@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>Lais Henriques de Mattos</t>
+          <t>Gabriela Ferreira Mota</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>laishenriques91@gmail.com</t>
+          <t>motafgabriela@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>Inês Corrêa Gonçalves</t>
+          <t>Ismar de Souza Carvalho</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>inescg.bio@gmail.com</t>
+          <t>ismar@geologia.ufrj.br</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>Lucas Pereira da Rocha</t>
+          <t>Clarice Assumpção da Costa</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>lucasrocha700@gmail.com</t>
+          <t>assumpcao.clarice@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>Alexandra Paris Toledo</t>
+          <t>Ingrid Martins Machado Garcia Veiga</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>alepariis@gmail.com</t>
+          <t>ingridgveiga@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>Alessandra Pavan Lamarca</t>
+          <t>Luiza Silva Anselmini</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>pavanlamarca@gmail.com</t>
+          <t>miniansel.lu@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>Luísa Andrade Mendes</t>
+          <t>Gabriela Mussalem Haddad</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>mendesluisa1997@gmail.com</t>
+          <t>gabimh3181@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>Melissa Bars Closel</t>
+          <t>Luísa Andrade Mendes</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>melissabars@gmail.com</t>
+          <t>mendesluisa1997@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>Breno Michelon Seixas</t>
+          <t>Lais Henriques de Mattos</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>breno.mseixas@usp.br</t>
+          <t>laishenriques91@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>Martín Rodrigo Escobar</t>
+          <t>Inês Corrêa Gonçalves</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>martin.escobar@usp.br</t>
+          <t>inescg.bio@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>Thiago Takeshi Goto</t>
+          <t>ALENA MAYO INIGUEZ</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>thi.takeshi@gmail.com</t>
+          <t>alenainiguez@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>Danilo Camargo Fernandes</t>
+          <t>Lucas Pereira da Rocha</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>danilo.fernandes@usp.br</t>
+          <t>lucasrocha700@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>Lucas Barcelos</t>
+          <t>Alessandra Pavan Lamarca</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>lucasabarcelos@gmail.com</t>
+          <t>pavanlamarca@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>Lígia Mouriño de Almeida Prado</t>
+          <t>Alexandra Paris Toledo</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>ligia.prado@unesp.br</t>
+          <t>alepariis@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>Ana Malaghini de Abreu</t>
+          <t>Melissa Bars Closel</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>anamalaghini9gold@gmail.com</t>
+          <t>melissabars@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Gabriel Tofanelo Vanin</t>
+          <t>Breno Michelon Seixas</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>gabriel.vanin@unesp.br</t>
+          <t>breno.mseixas@usp.br</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>Gustavo da Silva Ambrosio</t>
+          <t>Martín Rodrigo Escobar</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>gustavo.ambrosio@unesp.br</t>
+          <t>martin.escobar@usp.br</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>Fernanda Biscaino Saluceste</t>
+          <t>Danilo Camargo Fernandes</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>fernanda.saluceste@unesp.br</t>
+          <t>danilo.fernandes@usp.br</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>Leonardo Maurici Borges</t>
+          <t>Thiago Takeshi Goto</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>aquitemcaqui@gmail.com</t>
+          <t>thi.takeshi@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>Rafael Fernandes Barduzzi</t>
+          <t>Lucas Barcelos</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>rfbarduzzi@gmail.com</t>
+          <t>lucasabarcelos@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>Lucas Pereira Camargo</t>
+          <t>Lígia Mouriño de Almeida Prado</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>lucaspc@estudante.ufscar.br</t>
+          <t>ligia.prado@unesp.br</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>João Pedro Fujita</t>
+          <t>Ana Malaghini de Abreu</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>joaopedrofujita@estudante.ufscar.br</t>
+          <t>anamalaghini9gold@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Victor Hugo Barbosa Pereira</t>
+          <t>Gabriel Tofanelo Vanin</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>vhb.pereira@unesp.br</t>
+          <t>gabriel.vanin@unesp.br</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>Francisco Borges</t>
+          <t>Gustavo da Silva Ambrosio</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>fa.borges@unesp.br</t>
+          <t>gustavo.ambrosio@unesp.br</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>João Francisco Ponticelli Tottene</t>
+          <t>Fernanda Biscaino Saluceste</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>tott.joao@gmail.com</t>
+          <t>fernanda.saluceste@unesp.br</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>Felipe Messias Leandro</t>
+          <t>Leonardo Maurici Borges</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>felipe.messias@unesp.br</t>
+          <t>aquitemcaqui@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>Analice Gabrielle Marquezin Gomes</t>
+          <t>Rafael Fernandes Barduzzi</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>analice.gabrielle@unesp.br</t>
+          <t>rfbarduzzi@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>Luiza de Moraes Magaldi</t>
+          <t>Lucas Pereira Camargo</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>luiza.magaldi@gmail.com</t>
+          <t>lucaspc@estudante.ufscar.br</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>João Claudio de Sousa Nascimento</t>
+          <t>João Pedro Fujita</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>j.claudionasci@gmail.com</t>
+          <t>joaopedrofujita@estudante.ufscar.br</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>Pábulo Matheus Domiciano</t>
+          <t>Francisco Borges</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>pabulodomiciano@gmail.com</t>
+          <t>fa.borges@unesp.br</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>Nicolle Souza Leto</t>
+          <t>João Francisco Ponticelli Tottene</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>letonicolle@gmail.com</t>
+          <t>tott.joao@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>Pedro Henrique Pacheco Mosquini</t>
+          <t>Felipe Messias Leandro</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>mosquiniphp@gmail.com</t>
+          <t>felipe.messias@unesp.br</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>Tami da Costa Cacossi</t>
+          <t>Victor Hugo Barbosa Pereira</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>tamiccacossi@gmail.com</t>
+          <t>vhb.pereira@unesp.br</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>Leonardo Duarte Santos</t>
+          <t>Analice Gabrielle Marquezin Gomes</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>santosldbio@gmail.com</t>
+          <t>analice.gabrielle@unesp.br</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>Vera Nisaka Solferini</t>
+          <t>Lina Maria Ameida Silva</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>veras@unicamp.br</t>
+          <t>linamas@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>Julia Nader Acquaviva</t>
+          <t>Amanda Lichtscheidl Graciadio</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>julianader95@gmail.com</t>
+          <t>a265805@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>Henrique Vilela da Mata Bianchini</t>
+          <t>Pedro Danel de Souza Ugarte</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>h236891@dac.unicamp.br</t>
+          <t>pedaugaso@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>Paulo Aecyo Francisco da Silva</t>
+          <t>Beatriz Helena Macari Daros</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>pauloaecyo_1997@hotmail.com</t>
+          <t>beatrizdarosbio@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>Beatriz Helena Macari Daros</t>
+          <t>Paulo Aecyo Francisco da Silva</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>beatrizdarosbio@gmail.com</t>
+          <t>pauloaecyo_1997@hotmail.com</t>
         </is>
       </c>
     </row>
@@ -3720,514 +3720,634 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>Pedro Danel de Souza Ugarte</t>
+          <t>Lucas Albuquerque dos Santos</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>pedaugaso@gmail.com</t>
+          <t>lucasabqsto@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>Lucas Albuquerque dos Santos</t>
+          <t>Luiza de Moraes Magaldi</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>lucasabqsto@gmail.com</t>
+          <t>luiza.magaldi@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>Amanda Lichtscheidl Graciadio</t>
+          <t>João Claudio de Sousa Nascimento</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>a265805@dac.unicamp.br</t>
+          <t>j.claudionasci@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>Tiago Benedito dos Santos</t>
+          <t>Fernando Sotero de Lara</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>tiagobio02@yahoo.com.br</t>
+          <t>f236823@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>Jardel De Oliveira</t>
+          <t>Pábulo Matheus Domiciano</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>jardel.oliveira90@hotmail.com</t>
+          <t>pabulodomiciano@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>Diliane Harumi Yaguinuma</t>
+          <t>Nicolle Souza Leto</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>diliane-harumi@hotmail.com</t>
+          <t>letonicolle@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>Ana Claudia Lessinger</t>
+          <t>Pedro Henrique Pacheco Mosquini</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>lessinger@ufscar.br</t>
+          <t>mosquiniphp@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>Miguel Piovesana Pereira Romeiro</t>
+          <t>Tami da Costa Cacossi</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>miguelpromeiro@gmail.com</t>
+          <t>tamiccacossi@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>Eduardo Koerich Nery</t>
+          <t>Leonardo Duarte Santos</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>eduardo.k.nery@gmail.com</t>
+          <t>santosldbio@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>Irene De Fátima Vieira De Moraes</t>
+          <t>Isa Eloá de Freitas Poloni</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>irenef.vieiram@gmail.com</t>
+          <t>isaeloa011203@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>Ana Paula Becker</t>
+          <t>Vera Nisaka Solferini</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>ana.becker023@gmail.com</t>
+          <t>veras@unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>Marcelo Duarte</t>
+          <t>Julia Nader Acquaviva</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>mduartes@usp.br</t>
+          <t>julianader95@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>Rafaela Velloso Missagia</t>
+          <t>Henrique Vilela da Mata Bianchini</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>rafaelamissagia@gmail.com</t>
+          <t>h236891@dac.unicamp.br</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>Diogo Melo</t>
+          <t>Diliane Harumi Yaguinuma</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>diogro@gmail.com</t>
+          <t>diliane-harumi@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>Weverton dos Santos Azevedo</t>
+          <t>Jardel De Oliveira</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>weverton.azevedo@hotmail.com</t>
+          <t>jardel.oliveira90@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>Ana Paula Assis</t>
+          <t>Tiago Benedito dos Santos</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>paulaassis@ib.usp.br</t>
+          <t>tiagobio02@yahoo.com.br</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>Joyce Rodrigues do Prado</t>
+          <t>Ana Claudia Lessinger</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>joyce.prado@usp.br</t>
+          <t>lessinger@ufscar.br</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>Samuel Augusto Aguiar dos Anjos</t>
+          <t>Miguel Piovesana Pereira Romeiro</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>sam_aanjos@usp.br</t>
+          <t>miguelpromeiro@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>katarine nogueira norbertino</t>
+          <t>Eduardo Koerich Nery</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>katarinenn@outlook.com</t>
+          <t>eduardo.k.nery@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>Letícia Wanderley Cavalcanti</t>
+          <t>Irene De Fátima Vieira De Moraes</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>letcavalcanti02@gmail.com</t>
+          <t>irenef.vieiram@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>Tábita Hünemeier</t>
+          <t>Ana Paula Becker</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>hunemeier@usp.br</t>
+          <t>ana.becker023@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>Gabriela Procópio Camacho</t>
+          <t>Marcelo Duarte</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>gpcamacho@usp.br</t>
+          <t>mduartes@usp.br</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>Thiago Silva Loboda</t>
+          <t>Weverton dos Santos Azevedo</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>loboda_bio@yahoo.com.br</t>
+          <t>weverton.azevedo@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>Nathália Caldeira Dias</t>
+          <t>Rafaela Velloso Missagia</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>caldeira.nathalia@gmail.com</t>
+          <t>rafaelamissagia@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>Carlos Cristiano Simões Ferreira e Penha</t>
+          <t>Diogo Melo</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>cristianosf@usp.br</t>
+          <t>diogro@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>Denis Calandriello Calio</t>
+          <t>Ana Paula Assis</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>denis.calan@gmail.com</t>
+          <t>paulaassis@ib.usp.br</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>Tiago Bosisio Quental</t>
+          <t>Joyce Rodrigues do Prado</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>tbquental@usp.br</t>
+          <t>joyce.prado@usp.br</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>AMMIR YACOUB HELOU</t>
+          <t>katarine nogueira norbertino</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>ammir@usp.br</t>
+          <t>katarinenn@outlook.com</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>Ivan Sergio Nunes Silva Filho</t>
+          <t>Samuel Augusto Aguiar dos Anjos</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>ivan.nunes@unesp.br</t>
+          <t>sam_aanjos@usp.br</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>Alexander Tamanini Mônico</t>
+          <t>Letícia Wanderley Cavalcanti</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>alexandermonico@hotmail.com</t>
+          <t>letcavalcanti02@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>Fernanda de Pinho Werneck</t>
+          <t>Tábita Hünemeier</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>fewerneck@gmail.com</t>
+          <t>hunemeier@usp.br</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>Erik Henrique de Lacerda Choueri</t>
+          <t>Gabriela Procópio Camacho</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>chouerik@gmail.com</t>
+          <t>gpcamacho@usp.br</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>Esteban Diego Koch</t>
+          <t>Thiago Silva Loboda</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>edkoch17@gmail.com</t>
+          <t>loboda_bio@yahoo.com.br</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>Frederico Felizardo Barbosa</t>
+          <t>Nathália Caldeira Dias</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>fredericofb012@gmail.com</t>
+          <t>caldeira.nathalia@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>Amanda Freitas Haase</t>
+          <t>Denis Calandriello Calio</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>amandafreitashaase@gmail.com</t>
+          <t>denis.calan@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>Felipe Arian de Andrade Araújo</t>
+          <t>Carlos Cristiano Simões Ferreira e Penha</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>araujo.felipearian@gmail.com</t>
+          <t>cristianosf@usp.br</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>Gilmax Gonçalves Ferreira</t>
+          <t>Tiago Bosisio Quental</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>gillmax88@gmail.com</t>
+          <t>tbquental@usp.br</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>Thais Helena Condez</t>
+          <t>AMMIR YACOUB HELOU</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>thacondez@gmail.com</t>
+          <t>ammir@usp.br</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>Pamela Maciel Cremonez</t>
+          <t>Ivan Sergio Nunes Silva Filho</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>pamelacremonez@gmail.com</t>
+          <t>ivan.nunes@unesp.br</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>Isabella Fagundes Rosa Limão</t>
+          <t>Fernanda de Pinho Werneck</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>isaarlimao@gmail.com</t>
+          <t>fewerneck@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>Jonas Conduru Barros Neto</t>
+          <t>Erik Henrique de Lacerda Choueri</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>jonas.barrosneto@discente.univasf.edu.br</t>
+          <t>chouerik@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>Gabriela Procopio Leite</t>
+          <t>Alexander Tamanini Mônico</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>gabrielaprocopio3@gmail.com</t>
+          <t>alexandermonico@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
+          <t>Esteban Diego Koch</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>edkoch17@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>Frederico Felizardo Barbosa</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>fredericofb012@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>Amanda Freitas Haase</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>amandafreitashaase@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>Felipe Arian de Andrade Araújo</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>araujo.felipearian@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>Gilmax Gonçalves Ferreira</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>gillmax88@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>Thais Helena Condez</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>thacondez@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>Pamela Maciel Cremonez</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>pamelacremonez@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>Isabella Fagundes Rosa Limão</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>isaarlimao@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>Jonas Conduru Barros Neto</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>jonas.barrosneto@discente.univasf.edu.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>Gabriela Procopio Leite</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>gabrielaprocopio3@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
           <t>Jonathan Murilo Andreu Conrado</t>
         </is>
       </c>
-      <c r="B323" t="inlineStr">
+      <c r="B333" t="inlineStr">
         <is>
           <t>jonathan.conrajo@gmail.com</t>
         </is>

</xml_diff>